<commit_message>
updated the data.xlsx to read the data from excel duing new user signup
</commit_message>
<xml_diff>
--- a/BestbuyDDFramework/data.xlsx
+++ b/BestbuyDDFramework/data.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace3\BestbuyDDFramework\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="12810"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10905" windowHeight="6495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>computer</t>
   </si>
@@ -127,19 +123,62 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>newpassword</t>
+  </si>
+  <si>
+    <t>confirmpassword</t>
+  </si>
+  <si>
+    <t>Testing5</t>
+  </si>
+  <si>
+    <t>Testing5@gmail.com</t>
+  </si>
+  <si>
+    <t>Creating New Account</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Testing4@gmail.com</t>
+  </si>
+  <si>
+    <t>Newuser</t>
+  </si>
+  <si>
+    <t>Registereduser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,17 +198,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -450,11 +495,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -646,14 +694,14 @@
       <c r="O16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P16" s="1"/>
+      <c r="P16" s="3"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -661,49 +709,107 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
       <c r="L21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M21" s="1"/>
+      <c r="M21" s="3"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23">
+        <v>8056037388</v>
+      </c>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="L21:M29"/>
     <mergeCell ref="O16:P17"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C23" r:id="rId1"/>
+    <hyperlink ref="A28" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data.xlsx changed in kannan reop
</commit_message>
<xml_diff>
--- a/BestbuyDDFramework/data.xlsx
+++ b/BestbuyDDFramework/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace3\BestbuyDDFramework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspacebranch\BestbuyDDFramework\BestbuyDDFramework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>computer</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>checkBoxVerification</t>
+  </si>
+  <si>
+    <t>tablet</t>
   </si>
 </sst>
 </file>
@@ -164,10 +170,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,10 +457,13 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -643,60 +652,71 @@
       <c r="B16" t="s">
         <v>3</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="O16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P16" s="1"/>
+      <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L21" s="2" t="s">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M21" s="1"/>
+      <c r="M21" s="2"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
updated the data excel to incorporate 3 testcases
</commit_message>
<xml_diff>
--- a/BestbuyDDFramework/data.xlsx
+++ b/BestbuyDDFramework/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10905" windowHeight="6495"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11025" windowHeight="6495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -496,7 +496,7 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>